<commit_message>
leer estilos e insertarlos
</commit_message>
<xml_diff>
--- a/salida/salida1.xlsx
+++ b/salida/salida1.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Edad</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>edad</t>
   </si>
   <si>
     <t>1</t>

</xml_diff>